<commit_message>
- Actualización validaciones NIC para Costa Rica - Actualización de templates
</commit_message>
<xml_diff>
--- a/Template/Export/Sari_Cases_11.xlsx
+++ b/Template/Export/Sari_Cases_11.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Template\Export\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4743D58B-EF31-4C01-A3D4-2C0771F0E2E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10215"/>
   </bookViews>
   <sheets>
     <sheet name="export" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="278">
   <si>
     <t>ID</t>
   </si>
@@ -847,20 +846,35 @@
   </si>
   <si>
     <t>process6_other2_virus</t>
+  </si>
+  <si>
+    <t>Asymptomatic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rhinorrhoea </t>
+  </si>
+  <si>
+    <t>Odinophagia</t>
+  </si>
+  <si>
+    <t>Anosmy</t>
+  </si>
+  <si>
+    <t>Dysgeusia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="dd/mmm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="[$-409]dd/mmm/yyyy;@"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="yyyy/mm/dd"/>
-    <numFmt numFmtId="169" formatCode="[$-40A]dd/mmmm/yyyy;@"/>
+    <numFmt numFmtId="168" formatCode="[$-40A]dd/mmmm/yyyy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -871,6 +885,21 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -921,38 +950,70 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -971,7 +1032,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1046,23 +1107,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1098,23 +1142,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1290,32 +1317,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:JN10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:JS10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="6" customWidth="1"/>
     <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" style="11" customWidth="1"/>
-    <col min="15" max="15" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18" style="6" customWidth="1"/>
+    <col min="15" max="15" width="6.42578125" customWidth="1"/>
+    <col min="16" max="16" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="12.28515625" bestFit="1" customWidth="1"/>
@@ -1352,13 +1379,13 @@
     <col min="53" max="53" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="17" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="15" style="11" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="15" style="6" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="17.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="13.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="13.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="63" max="63" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="10" customWidth="1"/>
     <col min="65" max="65" width="15.140625" bestFit="1" customWidth="1"/>
@@ -1377,1060 +1404,1080 @@
     <col min="78" max="78" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="79" max="79" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="80" max="80" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="16" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="14.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="12" customWidth="1"/>
-    <col min="98" max="98" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="19" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="25" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="16" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="9.5703125" customWidth="1"/>
-    <col min="118" max="118" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="124" max="124" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="125" max="125" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="127" max="127" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="128" max="128" width="15.42578125" customWidth="1"/>
-    <col min="129" max="129" width="14.5703125" style="11" customWidth="1"/>
-    <col min="130" max="130" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="131" max="131" width="18.85546875" style="11" customWidth="1"/>
-    <col min="132" max="132" width="19" bestFit="1" customWidth="1"/>
-    <col min="133" max="133" width="22" style="11" customWidth="1"/>
-    <col min="134" max="134" width="6.42578125" style="11" customWidth="1"/>
-    <col min="135" max="135" width="13.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="136" max="136" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="137" max="137" width="18.28515625" style="11" customWidth="1"/>
-    <col min="138" max="138" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="139" max="139" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="140" max="140" width="11.28515625" customWidth="1"/>
-    <col min="141" max="141" width="14.140625" customWidth="1"/>
-    <col min="142" max="142" width="11.85546875" customWidth="1"/>
-    <col min="143" max="143" width="14" customWidth="1"/>
-    <col min="144" max="144" width="12.140625" style="9" customWidth="1"/>
-    <col min="145" max="145" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="146" max="146" width="19.140625" style="1" customWidth="1"/>
-    <col min="147" max="147" width="24.5703125" style="1" customWidth="1"/>
-    <col min="148" max="148" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="149" max="149" width="21.42578125" customWidth="1"/>
-    <col min="150" max="150" width="13.140625" style="11" customWidth="1"/>
-    <col min="151" max="151" width="12.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="152" max="152" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="153" max="153" width="12.140625" style="11" customWidth="1"/>
-    <col min="154" max="154" width="18.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="155" max="155" width="20" style="11" customWidth="1"/>
-    <col min="156" max="156" width="10" style="9" bestFit="1" customWidth="1"/>
-    <col min="157" max="157" width="16.7109375" style="7" customWidth="1"/>
-    <col min="158" max="158" width="18.85546875" style="6" customWidth="1"/>
-    <col min="159" max="159" width="21.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="160" max="160" width="24.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="161" max="161" width="16.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="162" max="162" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="163" max="163" width="14.7109375" style="9" customWidth="1"/>
-    <col min="164" max="164" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="165" max="165" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="166" max="166" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="167" max="167" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="168" max="168" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="169" max="169" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="170" max="170" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="171" max="171" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="172" max="172" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="22" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="16.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="7" style="1" customWidth="1"/>
+    <col min="95" max="95" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="21" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="15" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="11" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="26" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="8" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="18" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="20" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="127" max="127" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="129" max="129" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="130" max="130" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="131" max="131" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="15.42578125" customWidth="1"/>
+    <col min="134" max="134" width="14.5703125" style="6" customWidth="1"/>
+    <col min="135" max="135" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="136" max="136" width="18.85546875" style="6" customWidth="1"/>
+    <col min="137" max="137" width="19" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="22" style="6" customWidth="1"/>
+    <col min="139" max="139" width="6.42578125" style="6" customWidth="1"/>
+    <col min="140" max="140" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="141" max="141" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="142" max="142" width="18.28515625" style="6" customWidth="1"/>
+    <col min="143" max="143" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="144" max="144" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="145" max="145" width="11.28515625" customWidth="1"/>
+    <col min="146" max="146" width="14.140625" customWidth="1"/>
+    <col min="147" max="147" width="11.85546875" customWidth="1"/>
+    <col min="148" max="148" width="14" customWidth="1"/>
+    <col min="149" max="149" width="12.140625" style="5" customWidth="1"/>
+    <col min="150" max="150" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="151" max="151" width="19.140625" style="1" customWidth="1"/>
+    <col min="152" max="152" width="24.5703125" style="1" customWidth="1"/>
+    <col min="153" max="153" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="154" max="154" width="21.42578125" customWidth="1"/>
+    <col min="155" max="155" width="13.140625" style="6" customWidth="1"/>
+    <col min="156" max="156" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="157" max="157" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="158" max="158" width="12.140625" style="6" customWidth="1"/>
+    <col min="159" max="159" width="18.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="160" max="160" width="20" style="6" customWidth="1"/>
+    <col min="161" max="161" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="162" max="162" width="16.7109375" style="4" customWidth="1"/>
+    <col min="163" max="163" width="18.85546875" style="3" customWidth="1"/>
+    <col min="164" max="164" width="21.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="165" max="165" width="24.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="166" max="166" width="16.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="167" max="167" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="168" max="168" width="14.7109375" style="5" customWidth="1"/>
+    <col min="169" max="169" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="170" max="170" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="171" max="171" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="172" max="172" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="173" max="173" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="174" max="174" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="175" max="175" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="176" max="176" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="177" max="177" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="178" max="178" width="13.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="179" max="179" width="10.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="180" max="180" width="25.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="181" max="181" width="22.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="182" max="182" width="19.5703125" style="23" bestFit="1" customWidth="1"/>
-    <col min="183" max="183" width="18.7109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="184" max="184" width="15.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="185" max="185" width="16.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="186" max="186" width="15.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="187" max="188" width="15.42578125" style="22" customWidth="1"/>
-    <col min="189" max="189" width="18.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="190" max="190" width="17.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="191" max="191" width="16.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="192" max="192" width="9.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="193" max="193" width="25.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="194" max="194" width="22.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="195" max="195" width="20.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="196" max="196" width="19.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="197" max="197" width="15.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="198" max="198" width="15.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="199" max="199" width="17" style="22" bestFit="1" customWidth="1"/>
-    <col min="200" max="201" width="17" style="22" customWidth="1"/>
-    <col min="202" max="202" width="18.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="203" max="203" width="17.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="204" max="204" width="13.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="205" max="205" width="9.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="206" max="206" width="25.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="207" max="207" width="22.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="208" max="208" width="20" style="23" bestFit="1" customWidth="1"/>
-    <col min="209" max="209" width="19.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="210" max="210" width="14.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="211" max="211" width="15.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="212" max="212" width="14.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="213" max="214" width="14.7109375" style="22" customWidth="1"/>
-    <col min="215" max="215" width="17.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="216" max="216" width="17.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="217" max="217" width="13.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="218" max="218" width="9.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="219" max="219" width="25.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="220" max="220" width="22.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="221" max="221" width="20" style="23" bestFit="1" customWidth="1"/>
-    <col min="222" max="222" width="19.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="223" max="223" width="14.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="224" max="224" width="15.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="225" max="225" width="14.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="226" max="227" width="14.7109375" style="22" customWidth="1"/>
-    <col min="228" max="228" width="17.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="229" max="229" width="17.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="230" max="230" width="13.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="231" max="231" width="9.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="232" max="232" width="25.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="233" max="233" width="22.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="234" max="234" width="20" style="23" bestFit="1" customWidth="1"/>
-    <col min="235" max="235" width="19.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="236" max="236" width="14.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="237" max="237" width="15.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="238" max="238" width="14.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="239" max="240" width="14.7109375" style="22" customWidth="1"/>
-    <col min="241" max="241" width="17.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="242" max="242" width="17.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="243" max="243" width="13.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="244" max="244" width="9.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="245" max="245" width="25.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="246" max="246" width="22.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="247" max="247" width="20" style="23" bestFit="1" customWidth="1"/>
-    <col min="248" max="248" width="19.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="249" max="249" width="14.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="250" max="250" width="15.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="251" max="251" width="14.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="252" max="253" width="14.7109375" style="22" customWidth="1"/>
-    <col min="254" max="254" width="17.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="255" max="255" width="17.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="256" max="256" width="19.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="257" max="257" width="15.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="258" max="258" width="22.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="259" max="259" width="20" style="7" bestFit="1" customWidth="1"/>
-    <col min="260" max="260" width="19.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="261" max="261" width="22" style="7" bestFit="1" customWidth="1"/>
-    <col min="262" max="262" width="20" style="7" bestFit="1" customWidth="1"/>
-    <col min="263" max="263" width="17.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="264" max="264" width="23.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="265" max="265" width="10.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="266" max="266" width="17.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="267" max="267" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="268" max="268" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="269" max="269" width="20.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="270" max="270" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="271" max="271" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="272" max="272" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="273" max="273" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="274" max="275" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="276" max="276" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="278" max="278" width="24" customWidth="1"/>
+    <col min="176" max="176" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="177" max="177" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="178" max="178" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="179" max="179" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="180" max="180" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="181" max="181" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="182" max="182" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="183" max="183" width="13.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="184" max="184" width="10.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="185" max="185" width="25.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="186" max="186" width="22.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="187" max="187" width="19.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="188" max="188" width="18.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="189" max="189" width="15.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="190" max="190" width="16.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="191" max="191" width="15.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="192" max="193" width="15.42578125" style="7" customWidth="1"/>
+    <col min="194" max="194" width="18.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="195" max="195" width="17.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="196" max="196" width="16.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="197" max="197" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="198" max="198" width="25.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="199" max="199" width="22.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="200" max="200" width="20.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="201" max="201" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="202" max="202" width="15.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="203" max="203" width="15.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="204" max="204" width="17" style="7" bestFit="1" customWidth="1"/>
+    <col min="205" max="206" width="17" style="7" customWidth="1"/>
+    <col min="207" max="207" width="18.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="208" max="208" width="17.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="209" max="209" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="210" max="210" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="211" max="211" width="25.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="212" max="212" width="22.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="213" max="213" width="20" style="8" bestFit="1" customWidth="1"/>
+    <col min="214" max="214" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="215" max="215" width="14.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="216" max="216" width="15.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="217" max="217" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="218" max="219" width="14.7109375" style="7" customWidth="1"/>
+    <col min="220" max="220" width="17.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="221" max="221" width="17.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="222" max="222" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="223" max="223" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="224" max="224" width="25.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="225" max="225" width="22.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="226" max="226" width="20" style="8" bestFit="1" customWidth="1"/>
+    <col min="227" max="227" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="228" max="228" width="14.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="229" max="229" width="15.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="230" max="230" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="231" max="232" width="14.7109375" style="7" customWidth="1"/>
+    <col min="233" max="233" width="17.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="234" max="234" width="17.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="235" max="235" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="236" max="236" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="237" max="237" width="25.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="238" max="238" width="22.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="239" max="239" width="20" style="8" bestFit="1" customWidth="1"/>
+    <col min="240" max="240" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="241" max="241" width="14.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="242" max="242" width="15.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="243" max="243" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="244" max="245" width="14.7109375" style="7" customWidth="1"/>
+    <col min="246" max="246" width="17.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="247" max="247" width="17.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="248" max="248" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="249" max="249" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="250" max="250" width="25.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="251" max="251" width="22.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="252" max="252" width="20" style="8" bestFit="1" customWidth="1"/>
+    <col min="253" max="253" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="254" max="254" width="14.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="255" max="255" width="15.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="256" max="256" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="257" max="258" width="14.7109375" style="7" customWidth="1"/>
+    <col min="259" max="259" width="17.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="260" max="260" width="17.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="261" max="261" width="19.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="262" max="262" width="15.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="263" max="263" width="22.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="264" max="264" width="20" style="4" bestFit="1" customWidth="1"/>
+    <col min="265" max="265" width="19.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="266" max="266" width="22" style="4" bestFit="1" customWidth="1"/>
+    <col min="267" max="267" width="20" style="4" bestFit="1" customWidth="1"/>
+    <col min="268" max="268" width="17.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="269" max="269" width="23.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="270" max="270" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="271" max="271" width="17.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="272" max="272" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="273" max="273" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="274" max="274" width="20.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="275" max="275" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="276" max="276" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="277" max="277" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="278" max="278" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="279" max="280" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="281" max="281" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="283" max="283" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:274" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:279" s="26" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="S1" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="T1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="U1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="12" t="s">
+      <c r="V1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="12" t="s">
+      <c r="W1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="10" t="s">
         <v>249</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA1" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AB1" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="AC1" s="12" t="s">
+      <c r="AC1" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AD1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AE1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AF1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AG1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="AH1" s="12" t="s">
+      <c r="AH1" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AI1" s="12" t="s">
+      <c r="AI1" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="AJ1" s="12" t="s">
+      <c r="AJ1" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="AK1" s="12" t="s">
+      <c r="AK1" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="AL1" s="12" t="s">
+      <c r="AL1" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="AM1" s="12" t="s">
+      <c r="AM1" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="AN1" s="12" t="s">
+      <c r="AN1" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="AO1" s="12" t="s">
+      <c r="AO1" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="AP1" s="12" t="s">
+      <c r="AP1" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="AQ1" s="12" t="s">
+      <c r="AQ1" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="AR1" s="12" t="s">
+      <c r="AR1" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="AS1" s="12" t="s">
+      <c r="AS1" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="AT1" s="12" t="s">
+      <c r="AT1" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="AU1" s="12" t="s">
+      <c r="AU1" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="AV1" s="12" t="s">
+      <c r="AV1" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="AW1" s="12" t="s">
+      <c r="AW1" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="AX1" s="12" t="s">
+      <c r="AX1" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="AY1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="AZ1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BA1" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BB1" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="BC1" s="2" t="s">
+      <c r="BC1" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="BD1" s="8" t="s">
+      <c r="BD1" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="BE1" s="3" t="s">
+      <c r="BE1" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="BF1" s="2" t="s">
+      <c r="BF1" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="BG1" s="8" t="s">
+      <c r="BG1" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="BH1" s="2" t="s">
+      <c r="BH1" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="BI1" s="2" t="s">
+      <c r="BI1" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="BJ1" s="14" t="s">
+      <c r="BJ1" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="BK1" s="2" t="s">
+      <c r="BK1" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="BL1" s="2" t="s">
+      <c r="BL1" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="BM1" s="2" t="s">
+      <c r="BM1" s="10" t="s">
         <v>252</v>
       </c>
-      <c r="BN1" s="2" t="s">
+      <c r="BN1" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="BO1" s="2" t="s">
+      <c r="BO1" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="BP1" s="2" t="s">
+      <c r="BP1" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="BQ1" s="2" t="s">
+      <c r="BQ1" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="BR1" s="2" t="s">
+      <c r="BR1" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="BS1" s="2" t="s">
+      <c r="BS1" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="BT1" s="2" t="s">
+      <c r="BT1" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="BU1" s="2" t="s">
+      <c r="BU1" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="BV1" s="2" t="s">
+      <c r="BV1" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="BW1" s="2" t="s">
+      <c r="BW1" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="BX1" s="2" t="s">
+      <c r="BX1" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="BY1" s="2" t="s">
+      <c r="BY1" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="BZ1" s="12" t="s">
+      <c r="BZ1" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="CA1" s="12" t="s">
+      <c r="CA1" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="CB1" s="12" t="s">
+      <c r="CB1" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="CC1" s="2" t="s">
+      <c r="CC1" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="CD1" s="2" t="s">
+      <c r="CD1" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="CE1" s="2" t="s">
+      <c r="CE1" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="CF1" s="2" t="s">
+      <c r="CF1" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="CG1" s="2" t="s">
+      <c r="CG1" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="CH1" s="2" t="s">
+      <c r="CH1" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="CI1" s="2" t="s">
+      <c r="CI1" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="CJ1" s="2" t="s">
+      <c r="CJ1" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="CK1" s="2" t="s">
+      <c r="CK1" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="CL1" s="14" t="s">
+      <c r="CL1" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="CM1" s="5" t="s">
+      <c r="CM1" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="CN1" s="5" t="s">
+      <c r="CN1" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="CO1" s="2" t="s">
+      <c r="CO1" s="15" t="s">
+        <v>273</v>
+      </c>
+      <c r="CP1" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="CP1" s="12" t="s">
+      <c r="CQ1" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="CQ1" s="2" t="s">
+      <c r="CR1" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="CR1" s="2" t="s">
+      <c r="CS1" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="CS1" s="12" t="s">
+      <c r="CT1" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="CT1" s="12" t="s">
+      <c r="CU1" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="CU1" s="12" t="s">
+      <c r="CV1" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="CV1" s="12" t="s">
+      <c r="CW1" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="CW1" s="12" t="s">
+      <c r="CX1" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="CX1" s="12" t="s">
+      <c r="CY1" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="CY1" s="12" t="s">
+      <c r="CZ1" s="15" t="s">
+        <v>274</v>
+      </c>
+      <c r="DA1" s="15" t="s">
+        <v>275</v>
+      </c>
+      <c r="DB1" s="15" t="s">
+        <v>276</v>
+      </c>
+      <c r="DC1" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="DD1" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="CZ1" s="12" t="s">
+      <c r="DE1" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="DA1" s="12" t="s">
+      <c r="DF1" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="DB1" s="12" t="s">
+      <c r="DG1" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="DC1" s="12" t="s">
+      <c r="DH1" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="DD1" s="12" t="s">
+      <c r="DI1" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="DE1" s="12" t="s">
+      <c r="DJ1" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="DF1" s="12" t="s">
+      <c r="DK1" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="DG1" s="12" t="s">
+      <c r="DL1" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="DH1" s="12" t="s">
+      <c r="DM1" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="DI1" s="12" t="s">
+      <c r="DN1" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="DJ1" s="12" t="s">
+      <c r="DO1" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="DK1" s="12" t="s">
+      <c r="DP1" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="DL1" s="12" t="s">
+      <c r="DQ1" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="DM1" s="12" t="s">
+      <c r="DR1" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="DN1" s="12" t="s">
+      <c r="DS1" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="DO1" s="12" t="s">
+      <c r="DT1" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="DP1" s="12" t="s">
+      <c r="DU1" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="DQ1" s="12" t="s">
+      <c r="DV1" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="DR1" s="12" t="s">
+      <c r="DW1" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="DS1" s="12" t="s">
+      <c r="DX1" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="DT1" s="12" t="s">
+      <c r="DY1" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="DU1" s="12" t="s">
+      <c r="DZ1" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="DV1" s="12" t="s">
+      <c r="EA1" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="DW1" s="2" t="s">
+      <c r="EB1" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="DX1" s="2" t="s">
+      <c r="EC1" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="DY1" s="14" t="s">
+      <c r="ED1" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="DZ1" s="5" t="s">
+      <c r="EE1" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="EA1" s="14" t="s">
+      <c r="EF1" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="EB1" s="12" t="s">
+      <c r="EG1" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="EC1" s="15" t="s">
+      <c r="EH1" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="ED1" s="14" t="s">
+      <c r="EI1" s="17" t="s">
         <v>257</v>
       </c>
-      <c r="EE1" s="14" t="s">
+      <c r="EJ1" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="EF1" s="5" t="s">
+      <c r="EK1" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="EG1" s="14" t="s">
+      <c r="EL1" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="EH1" s="2" t="s">
+      <c r="EM1" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="EI1" s="14" t="s">
+      <c r="EN1" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="EJ1" s="8" t="s">
+      <c r="EO1" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="EK1" s="8" t="s">
+      <c r="EP1" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="EL1" s="4" t="s">
+      <c r="EQ1" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="EM1" s="4" t="s">
+      <c r="ER1" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="EN1" s="4" t="s">
+      <c r="ES1" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="EO1" s="2" t="s">
+      <c r="ET1" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="EP1" s="2" t="s">
+      <c r="EU1" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="EQ1" s="2" t="s">
+      <c r="EV1" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="ER1" s="14" t="s">
+      <c r="EW1" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="ES1" s="2" t="s">
+      <c r="EX1" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="ET1" s="14" t="s">
+      <c r="EY1" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="EU1" s="2" t="s">
+      <c r="EZ1" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="EV1" s="2" t="s">
+      <c r="FA1" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="EW1" s="14" t="s">
+      <c r="FB1" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="EX1" s="4" t="s">
+      <c r="FC1" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="EY1" s="18" t="s">
+      <c r="FD1" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="EZ1" s="19" t="s">
+      <c r="FE1" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="FA1" s="19" t="s">
+      <c r="FF1" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="FB1" s="19" t="s">
+      <c r="FG1" s="20" t="s">
         <v>256</v>
       </c>
-      <c r="FC1" s="19" t="s">
+      <c r="FH1" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="FD1" s="19" t="s">
+      <c r="FI1" s="20" t="s">
         <v>260</v>
       </c>
-      <c r="FE1" s="18" t="s">
+      <c r="FJ1" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="FF1" s="19" t="s">
+      <c r="FK1" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="FG1" s="16" t="s">
+      <c r="FL1" s="21" t="s">
         <v>237</v>
       </c>
-      <c r="FH1" s="16" t="s">
+      <c r="FM1" s="21" t="s">
         <v>238</v>
       </c>
-      <c r="FI1" s="16" t="s">
+      <c r="FN1" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="FJ1" s="16" t="s">
+      <c r="FO1" s="21" t="s">
         <v>240</v>
       </c>
-      <c r="FK1" s="16" t="s">
+      <c r="FP1" s="21" t="s">
         <v>253</v>
       </c>
-      <c r="FL1" s="17" t="s">
+      <c r="FQ1" s="22" t="s">
         <v>241</v>
       </c>
-      <c r="FM1" s="17" t="s">
+      <c r="FR1" s="22" t="s">
         <v>242</v>
       </c>
-      <c r="FN1" s="17" t="s">
+      <c r="FS1" s="22" t="s">
         <v>243</v>
       </c>
-      <c r="FO1" s="17" t="s">
+      <c r="FT1" s="22" t="s">
         <v>244</v>
       </c>
-      <c r="FP1" s="17" t="s">
+      <c r="FU1" s="22" t="s">
         <v>254</v>
       </c>
-      <c r="FQ1" s="16" t="s">
+      <c r="FV1" s="21" t="s">
         <v>245</v>
       </c>
-      <c r="FR1" s="16" t="s">
+      <c r="FW1" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="FS1" s="16" t="s">
+      <c r="FX1" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="FT1" s="16" t="s">
+      <c r="FY1" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="FU1" s="16" t="s">
+      <c r="FZ1" s="21" t="s">
         <v>255</v>
       </c>
-      <c r="FV1" s="20" t="s">
+      <c r="GA1" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="FW1" s="20" t="s">
+      <c r="GB1" s="23" t="s">
         <v>172</v>
       </c>
-      <c r="FX1" s="20" t="s">
+      <c r="GC1" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="FY1" s="20" t="s">
+      <c r="GD1" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="FZ1" s="21" t="s">
+      <c r="GE1" s="24" t="s">
         <v>175</v>
       </c>
-      <c r="GA1" s="20" t="s">
+      <c r="GF1" s="23" t="s">
         <v>176</v>
       </c>
-      <c r="GB1" s="20" t="s">
+      <c r="GG1" s="23" t="s">
         <v>177</v>
       </c>
-      <c r="GC1" s="20" t="s">
+      <c r="GH1" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="GD1" s="20" t="s">
+      <c r="GI1" s="23" t="s">
         <v>179</v>
       </c>
-      <c r="GE1" s="20" t="s">
+      <c r="GJ1" s="23" t="s">
         <v>261</v>
       </c>
-      <c r="GF1" s="20" t="s">
+      <c r="GK1" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="GG1" s="20" t="s">
+      <c r="GL1" s="23" t="s">
         <v>180</v>
       </c>
-      <c r="GH1" s="20" t="s">
+      <c r="GM1" s="23" t="s">
         <v>181</v>
       </c>
-      <c r="GI1" s="20" t="s">
+      <c r="GN1" s="23" t="s">
         <v>182</v>
       </c>
-      <c r="GJ1" s="20" t="s">
+      <c r="GO1" s="23" t="s">
         <v>183</v>
       </c>
-      <c r="GK1" s="20" t="s">
+      <c r="GP1" s="23" t="s">
         <v>184</v>
       </c>
-      <c r="GL1" s="20" t="s">
+      <c r="GQ1" s="23" t="s">
         <v>185</v>
       </c>
-      <c r="GM1" s="21" t="s">
+      <c r="GR1" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="GN1" s="20" t="s">
+      <c r="GS1" s="23" t="s">
         <v>187</v>
       </c>
-      <c r="GO1" s="20" t="s">
+      <c r="GT1" s="23" t="s">
         <v>188</v>
       </c>
-      <c r="GP1" s="20" t="s">
+      <c r="GU1" s="23" t="s">
         <v>189</v>
       </c>
-      <c r="GQ1" s="20" t="s">
+      <c r="GV1" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="GR1" s="20" t="s">
+      <c r="GW1" s="23" t="s">
         <v>263</v>
       </c>
-      <c r="GS1" s="20" t="s">
+      <c r="GX1" s="23" t="s">
         <v>264</v>
       </c>
-      <c r="GT1" s="20" t="s">
+      <c r="GY1" s="23" t="s">
         <v>191</v>
       </c>
-      <c r="GU1" s="20" t="s">
+      <c r="GZ1" s="23" t="s">
         <v>192</v>
       </c>
-      <c r="GV1" s="20" t="s">
+      <c r="HA1" s="23" t="s">
         <v>193</v>
       </c>
-      <c r="GW1" s="20" t="s">
+      <c r="HB1" s="23" t="s">
         <v>194</v>
       </c>
-      <c r="GX1" s="20" t="s">
+      <c r="HC1" s="23" t="s">
         <v>195</v>
       </c>
-      <c r="GY1" s="20" t="s">
+      <c r="HD1" s="23" t="s">
         <v>196</v>
       </c>
-      <c r="GZ1" s="21" t="s">
+      <c r="HE1" s="24" t="s">
         <v>197</v>
       </c>
-      <c r="HA1" s="20" t="s">
+      <c r="HF1" s="23" t="s">
         <v>198</v>
       </c>
-      <c r="HB1" s="20" t="s">
+      <c r="HG1" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="HC1" s="20" t="s">
+      <c r="HH1" s="23" t="s">
         <v>200</v>
       </c>
-      <c r="HD1" s="20" t="s">
+      <c r="HI1" s="23" t="s">
         <v>201</v>
       </c>
-      <c r="HE1" s="20" t="s">
+      <c r="HJ1" s="23" t="s">
         <v>265</v>
       </c>
-      <c r="HF1" s="20" t="s">
+      <c r="HK1" s="23" t="s">
         <v>266</v>
       </c>
-      <c r="HG1" s="20" t="s">
+      <c r="HL1" s="23" t="s">
         <v>202</v>
       </c>
-      <c r="HH1" s="20" t="s">
+      <c r="HM1" s="23" t="s">
         <v>203</v>
       </c>
-      <c r="HI1" s="20" t="s">
+      <c r="HN1" s="23" t="s">
         <v>204</v>
       </c>
-      <c r="HJ1" s="20" t="s">
+      <c r="HO1" s="23" t="s">
         <v>205</v>
       </c>
-      <c r="HK1" s="20" t="s">
+      <c r="HP1" s="23" t="s">
         <v>206</v>
       </c>
-      <c r="HL1" s="20" t="s">
+      <c r="HQ1" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="HM1" s="21" t="s">
+      <c r="HR1" s="24" t="s">
         <v>208</v>
       </c>
-      <c r="HN1" s="20" t="s">
+      <c r="HS1" s="23" t="s">
         <v>209</v>
       </c>
-      <c r="HO1" s="20" t="s">
+      <c r="HT1" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="HP1" s="20" t="s">
+      <c r="HU1" s="23" t="s">
         <v>211</v>
       </c>
-      <c r="HQ1" s="20" t="s">
+      <c r="HV1" s="23" t="s">
         <v>212</v>
       </c>
-      <c r="HR1" s="20" t="s">
+      <c r="HW1" s="23" t="s">
         <v>267</v>
       </c>
-      <c r="HS1" s="20" t="s">
+      <c r="HX1" s="23" t="s">
         <v>268</v>
       </c>
-      <c r="HT1" s="20" t="s">
+      <c r="HY1" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="HU1" s="20" t="s">
+      <c r="HZ1" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="HV1" s="20" t="s">
+      <c r="IA1" s="23" t="s">
         <v>215</v>
       </c>
-      <c r="HW1" s="20" t="s">
+      <c r="IB1" s="23" t="s">
         <v>216</v>
       </c>
-      <c r="HX1" s="20" t="s">
+      <c r="IC1" s="23" t="s">
         <v>217</v>
       </c>
-      <c r="HY1" s="20" t="s">
+      <c r="ID1" s="23" t="s">
         <v>218</v>
       </c>
-      <c r="HZ1" s="21" t="s">
+      <c r="IE1" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="IA1" s="20" t="s">
+      <c r="IF1" s="23" t="s">
         <v>220</v>
       </c>
-      <c r="IB1" s="20" t="s">
+      <c r="IG1" s="23" t="s">
         <v>221</v>
       </c>
-      <c r="IC1" s="20" t="s">
+      <c r="IH1" s="23" t="s">
         <v>222</v>
       </c>
-      <c r="ID1" s="20" t="s">
+      <c r="II1" s="23" t="s">
         <v>223</v>
       </c>
-      <c r="IE1" s="20" t="s">
+      <c r="IJ1" s="23" t="s">
         <v>269</v>
       </c>
-      <c r="IF1" s="20" t="s">
+      <c r="IK1" s="23" t="s">
         <v>270</v>
       </c>
-      <c r="IG1" s="20" t="s">
+      <c r="IL1" s="23" t="s">
         <v>224</v>
       </c>
-      <c r="IH1" s="20" t="s">
+      <c r="IM1" s="23" t="s">
         <v>225</v>
       </c>
-      <c r="II1" s="20" t="s">
+      <c r="IN1" s="23" t="s">
         <v>226</v>
       </c>
-      <c r="IJ1" s="20" t="s">
+      <c r="IO1" s="23" t="s">
         <v>227</v>
       </c>
-      <c r="IK1" s="20" t="s">
+      <c r="IP1" s="23" t="s">
         <v>228</v>
       </c>
-      <c r="IL1" s="20" t="s">
+      <c r="IQ1" s="23" t="s">
         <v>229</v>
       </c>
-      <c r="IM1" s="21" t="s">
+      <c r="IR1" s="24" t="s">
         <v>230</v>
       </c>
-      <c r="IN1" s="20" t="s">
+      <c r="IS1" s="23" t="s">
         <v>231</v>
       </c>
-      <c r="IO1" s="20" t="s">
+      <c r="IT1" s="23" t="s">
         <v>232</v>
       </c>
-      <c r="IP1" s="20" t="s">
+      <c r="IU1" s="23" t="s">
         <v>233</v>
       </c>
-      <c r="IQ1" s="20" t="s">
+      <c r="IV1" s="23" t="s">
         <v>234</v>
       </c>
-      <c r="IR1" s="20" t="s">
+      <c r="IW1" s="23" t="s">
         <v>271</v>
       </c>
-      <c r="IS1" s="20" t="s">
+      <c r="IX1" s="23" t="s">
         <v>272</v>
       </c>
-      <c r="IT1" s="20" t="s">
+      <c r="IY1" s="23" t="s">
         <v>235</v>
       </c>
-      <c r="IU1" s="20" t="s">
+      <c r="IZ1" s="23" t="s">
         <v>236</v>
       </c>
-      <c r="IV1" s="13" t="s">
+      <c r="JA1" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="IW1" s="13" t="s">
+      <c r="JB1" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="IX1" s="13" t="s">
+      <c r="JC1" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="IY1" s="13" t="s">
+      <c r="JD1" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="IZ1" s="13" t="s">
+      <c r="JE1" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="JA1" s="13" t="s">
+      <c r="JF1" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="JB1" s="13" t="s">
+      <c r="JG1" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="JC1" s="13" t="s">
+      <c r="JH1" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="JD1" s="13" t="s">
+      <c r="JI1" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="JE1" s="13" t="s">
+      <c r="JJ1" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="JF1" s="13" t="s">
+      <c r="JK1" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="JG1" s="13" t="s">
+      <c r="JL1" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="JH1" s="13" t="s">
+      <c r="JM1" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="JI1" s="2" t="s">
+      <c r="JN1" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="JJ1" s="2" t="s">
+      <c r="JO1" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="JK1" s="2" t="s">
+      <c r="JP1" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="JL1" s="2" t="s">
+      <c r="JQ1" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="JM1" s="2" t="s">
+      <c r="JR1" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="JN1" s="2" t="s">
+      <c r="JS1" s="10" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="3" spans="1:274" x14ac:dyDescent="0.25">
-      <c r="FN3" s="2"/>
-      <c r="FO3" s="2"/>
-      <c r="FP3" s="2"/>
+    <row r="3" spans="1:279" x14ac:dyDescent="0.25">
+      <c r="FS3" s="2"/>
+      <c r="FT3" s="2"/>
+      <c r="FU3" s="2"/>
     </row>
-    <row r="5" spans="1:274" x14ac:dyDescent="0.25">
-      <c r="FZ5" s="24"/>
-      <c r="GA5" s="22"/>
+    <row r="5" spans="1:279" x14ac:dyDescent="0.25">
+      <c r="GE5" s="9"/>
+      <c r="GF5" s="7"/>
     </row>
-    <row r="6" spans="1:274" x14ac:dyDescent="0.25">
-      <c r="FZ6" s="24"/>
-      <c r="GA6" s="22"/>
+    <row r="6" spans="1:279" x14ac:dyDescent="0.25">
+      <c r="GE6" s="9"/>
+      <c r="GF6" s="7"/>
     </row>
-    <row r="7" spans="1:274" x14ac:dyDescent="0.25">
-      <c r="FZ7" s="24"/>
-      <c r="GA7" s="22"/>
+    <row r="7" spans="1:279" x14ac:dyDescent="0.25">
+      <c r="GE7" s="9"/>
+      <c r="GF7" s="7"/>
     </row>
-    <row r="8" spans="1:274" x14ac:dyDescent="0.25">
-      <c r="FZ8" s="24"/>
-      <c r="GA8" s="22"/>
-      <c r="GM8" s="22"/>
-      <c r="GN8" s="22"/>
-      <c r="GZ8" s="22"/>
-      <c r="HA8" s="22"/>
-      <c r="HM8" s="22"/>
-      <c r="HN8" s="22"/>
-      <c r="HZ8" s="22"/>
-      <c r="IA8" s="22"/>
-      <c r="IM8" s="22"/>
-      <c r="IN8" s="22"/>
+    <row r="8" spans="1:279" x14ac:dyDescent="0.25">
+      <c r="GE8" s="9"/>
+      <c r="GF8" s="7"/>
+      <c r="GR8" s="7"/>
+      <c r="GS8" s="7"/>
+      <c r="HE8" s="7"/>
+      <c r="HF8" s="7"/>
+      <c r="HR8" s="7"/>
+      <c r="HS8" s="7"/>
+      <c r="IE8" s="7"/>
+      <c r="IF8" s="7"/>
+      <c r="IR8" s="7"/>
+      <c r="IS8" s="7"/>
     </row>
-    <row r="9" spans="1:274" x14ac:dyDescent="0.25">
-      <c r="FZ9" s="24"/>
-      <c r="GA9" s="22"/>
+    <row r="9" spans="1:279" x14ac:dyDescent="0.25">
+      <c r="GE9" s="9"/>
+      <c r="GF9" s="7"/>
     </row>
-    <row r="10" spans="1:274" x14ac:dyDescent="0.25">
-      <c r="FZ10" s="24"/>
-      <c r="GA10" s="22"/>
+    <row r="10" spans="1:279" x14ac:dyDescent="0.25">
+      <c r="GE10" s="9"/>
+      <c r="GF10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- Actualización reporte CR Exportación de fallecidos COVID - Actualización templates exportación de casos
</commit_message>
<xml_diff>
--- a/Template/Export/Sari_Cases_11.xlsx
+++ b/Template/Export/Sari_Cases_11.xlsx
@@ -1,33 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Template\Export\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5625B3A8-4BFB-4428-B427-3C38FED01CAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10215"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="export" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="282">
   <si>
     <t>ID</t>
   </si>
@@ -861,12 +854,24 @@
   </si>
   <si>
     <t>Dysgeusia</t>
+  </si>
+  <si>
+    <t>death_total</t>
+  </si>
+  <si>
+    <t>condition_discharge_other_evolution</t>
+  </si>
+  <si>
+    <t>condition_discharge_date_evolution</t>
+  </si>
+  <si>
+    <t>condition_discharge_evolution</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="dd/mmm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="[$-409]dd/mmm/yyyy;@"/>
@@ -906,7 +911,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -937,6 +942,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -950,7 +961,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1014,6 +1025,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1032,7 +1047,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1107,6 +1122,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1142,6 +1174,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1317,15 +1366,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:JS10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:JW10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
@@ -1466,142 +1515,146 @@
     <col min="140" max="140" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="141" max="141" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="142" max="142" width="18.28515625" style="6" customWidth="1"/>
-    <col min="143" max="143" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="144" max="144" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="145" max="145" width="11.28515625" customWidth="1"/>
-    <col min="146" max="146" width="14.140625" customWidth="1"/>
-    <col min="147" max="147" width="11.85546875" customWidth="1"/>
-    <col min="148" max="148" width="14" customWidth="1"/>
-    <col min="149" max="149" width="12.140625" style="5" customWidth="1"/>
-    <col min="150" max="150" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="151" max="151" width="19.140625" style="1" customWidth="1"/>
-    <col min="152" max="152" width="24.5703125" style="1" customWidth="1"/>
-    <col min="153" max="153" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="154" max="154" width="21.42578125" customWidth="1"/>
-    <col min="155" max="155" width="13.140625" style="6" customWidth="1"/>
-    <col min="156" max="156" width="12.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="157" max="157" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="158" max="158" width="12.140625" style="6" customWidth="1"/>
-    <col min="159" max="159" width="18.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="160" max="160" width="20" style="6" customWidth="1"/>
-    <col min="161" max="161" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="162" max="162" width="16.7109375" style="4" customWidth="1"/>
-    <col min="163" max="163" width="18.85546875" style="3" customWidth="1"/>
-    <col min="164" max="164" width="21.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="165" max="165" width="24.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="166" max="166" width="16.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="167" max="167" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="168" max="168" width="14.7109375" style="5" customWidth="1"/>
-    <col min="169" max="169" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="170" max="170" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="171" max="171" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="172" max="172" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="173" max="173" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="174" max="174" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="175" max="175" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="176" max="176" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="177" max="177" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="178" max="178" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="179" max="179" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="180" max="180" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="181" max="181" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="182" max="182" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="183" max="183" width="13.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="184" max="184" width="10.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="185" max="185" width="25.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="186" max="186" width="22.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="187" max="187" width="19.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="188" max="188" width="18.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="189" max="189" width="15.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="190" max="190" width="16.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="191" max="191" width="15.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="192" max="193" width="15.42578125" style="7" customWidth="1"/>
-    <col min="194" max="194" width="18.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="195" max="195" width="17.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="196" max="196" width="16.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="197" max="197" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="198" max="198" width="25.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="199" max="199" width="22.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="200" max="200" width="20.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="201" max="201" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="202" max="202" width="15.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="203" max="203" width="15.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="204" max="204" width="17" style="7" bestFit="1" customWidth="1"/>
-    <col min="205" max="206" width="17" style="7" customWidth="1"/>
-    <col min="207" max="207" width="18.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="208" max="208" width="17.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="209" max="209" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="210" max="210" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="211" max="211" width="25.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="212" max="212" width="22.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="213" max="213" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="214" max="214" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="215" max="215" width="14.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="216" max="216" width="15.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="217" max="217" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="218" max="219" width="14.7109375" style="7" customWidth="1"/>
-    <col min="220" max="220" width="17.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="221" max="221" width="17.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="222" max="222" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="223" max="223" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="224" max="224" width="25.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="225" max="225" width="22.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="226" max="226" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="227" max="227" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="228" max="228" width="14.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="229" max="229" width="15.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="230" max="230" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="231" max="232" width="14.7109375" style="7" customWidth="1"/>
-    <col min="233" max="233" width="17.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="234" max="234" width="17.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="235" max="235" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="236" max="236" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="237" max="237" width="25.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="238" max="238" width="22.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="239" max="239" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="240" max="240" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="241" max="241" width="14.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="242" max="242" width="15.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="243" max="243" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="244" max="245" width="14.7109375" style="7" customWidth="1"/>
-    <col min="246" max="246" width="17.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="247" max="247" width="17.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="248" max="248" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="249" max="249" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="250" max="250" width="25.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="251" max="251" width="22.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="252" max="252" width="20" style="8" bestFit="1" customWidth="1"/>
-    <col min="253" max="253" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="254" max="254" width="14.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="255" max="255" width="15.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="256" max="256" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="257" max="258" width="14.7109375" style="7" customWidth="1"/>
-    <col min="259" max="259" width="17.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="260" max="260" width="17.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="261" max="261" width="19.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="262" max="262" width="15.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="263" max="263" width="22.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="264" max="264" width="20" style="4" bestFit="1" customWidth="1"/>
-    <col min="265" max="265" width="19.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="266" max="266" width="22" style="4" bestFit="1" customWidth="1"/>
-    <col min="267" max="267" width="20" style="4" bestFit="1" customWidth="1"/>
-    <col min="268" max="268" width="17.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="269" max="269" width="23.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="270" max="270" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="271" max="271" width="17.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="272" max="272" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="273" max="273" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="274" max="274" width="20.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="275" max="275" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="276" max="276" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="277" max="277" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="278" max="278" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="279" max="280" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="281" max="281" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="283" max="283" width="24" customWidth="1"/>
+    <col min="143" max="143" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="144" max="144" width="18.42578125" style="6" customWidth="1"/>
+    <col min="145" max="145" width="32.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="146" max="146" width="38.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="147" max="147" width="39.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="148" max="148" width="13.85546875" style="28" customWidth="1"/>
+    <col min="149" max="149" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="150" max="150" width="14.140625" customWidth="1"/>
+    <col min="151" max="151" width="11.85546875" customWidth="1"/>
+    <col min="152" max="152" width="14" customWidth="1"/>
+    <col min="153" max="153" width="12.140625" style="5" customWidth="1"/>
+    <col min="154" max="154" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="155" max="155" width="19.140625" style="1" customWidth="1"/>
+    <col min="156" max="156" width="24.5703125" style="1" customWidth="1"/>
+    <col min="157" max="157" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="158" max="158" width="21.42578125" customWidth="1"/>
+    <col min="159" max="159" width="13.140625" style="6" customWidth="1"/>
+    <col min="160" max="160" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="161" max="161" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="162" max="162" width="12.140625" style="6" customWidth="1"/>
+    <col min="163" max="163" width="18.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="164" max="164" width="20" style="6" customWidth="1"/>
+    <col min="165" max="165" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="166" max="166" width="16.7109375" style="4" customWidth="1"/>
+    <col min="167" max="167" width="18.85546875" style="3" customWidth="1"/>
+    <col min="168" max="168" width="21.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="169" max="169" width="24.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="170" max="170" width="16.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="171" max="171" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="172" max="172" width="14.7109375" style="5" customWidth="1"/>
+    <col min="173" max="173" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="174" max="174" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="175" max="175" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="176" max="176" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="177" max="177" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="178" max="178" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="179" max="179" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="180" max="180" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="181" max="181" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="182" max="182" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="183" max="183" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="184" max="184" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="185" max="185" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="186" max="186" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="187" max="187" width="13.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="188" max="188" width="10.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="189" max="189" width="25.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="190" max="190" width="22.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="191" max="191" width="19.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="192" max="192" width="18.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="193" max="193" width="15.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="194" max="194" width="16.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="195" max="195" width="15.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="196" max="197" width="15.42578125" style="7" customWidth="1"/>
+    <col min="198" max="198" width="18.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="199" max="199" width="17.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="200" max="200" width="16.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="201" max="201" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="202" max="202" width="25.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="203" max="203" width="22.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="204" max="204" width="20.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="205" max="205" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="206" max="206" width="15.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="207" max="207" width="15.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="208" max="208" width="17" style="7" bestFit="1" customWidth="1"/>
+    <col min="209" max="210" width="17" style="7" customWidth="1"/>
+    <col min="211" max="211" width="18.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="212" max="212" width="17.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="213" max="213" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="214" max="214" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="215" max="215" width="25.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="216" max="216" width="22.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="217" max="217" width="20" style="8" bestFit="1" customWidth="1"/>
+    <col min="218" max="218" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="219" max="219" width="14.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="220" max="220" width="15.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="221" max="221" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="222" max="223" width="14.7109375" style="7" customWidth="1"/>
+    <col min="224" max="224" width="17.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="225" max="225" width="17.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="226" max="226" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="227" max="227" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="228" max="228" width="25.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="229" max="229" width="22.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="230" max="230" width="20" style="8" bestFit="1" customWidth="1"/>
+    <col min="231" max="231" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="232" max="232" width="14.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="233" max="233" width="15.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="234" max="234" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="235" max="236" width="14.7109375" style="7" customWidth="1"/>
+    <col min="237" max="237" width="17.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="238" max="238" width="17.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="239" max="239" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="240" max="240" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="241" max="241" width="25.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="242" max="242" width="22.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="243" max="243" width="20" style="8" bestFit="1" customWidth="1"/>
+    <col min="244" max="244" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="245" max="245" width="14.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="246" max="246" width="15.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="247" max="247" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="248" max="249" width="14.7109375" style="7" customWidth="1"/>
+    <col min="250" max="250" width="17.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="251" max="251" width="17.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="252" max="252" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="253" max="253" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="254" max="254" width="25.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="255" max="255" width="22.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="256" max="256" width="20" style="8" bestFit="1" customWidth="1"/>
+    <col min="257" max="257" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="258" max="258" width="14.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="259" max="259" width="15.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="260" max="260" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="261" max="262" width="14.7109375" style="7" customWidth="1"/>
+    <col min="263" max="263" width="17.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="264" max="264" width="17.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="265" max="265" width="19.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="266" max="266" width="15.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="267" max="267" width="22.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="268" max="268" width="20" style="4" bestFit="1" customWidth="1"/>
+    <col min="269" max="269" width="19.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="270" max="270" width="22" style="4" bestFit="1" customWidth="1"/>
+    <col min="271" max="271" width="20" style="4" bestFit="1" customWidth="1"/>
+    <col min="272" max="272" width="17.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="273" max="273" width="23.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="274" max="274" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="275" max="275" width="17.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="276" max="276" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="277" max="277" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="278" max="278" width="20.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="279" max="279" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="280" max="280" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="281" max="281" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="282" max="282" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="283" max="284" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="285" max="285" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="287" max="287" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:279" s="26" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:283" s="26" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -2034,450 +2087,462 @@
       <c r="EN1" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="EO1" s="11" t="s">
+      <c r="EO1" s="23" t="s">
+        <v>281</v>
+      </c>
+      <c r="EP1" s="23" t="s">
+        <v>280</v>
+      </c>
+      <c r="EQ1" s="23" t="s">
+        <v>279</v>
+      </c>
+      <c r="ER1" s="27" t="s">
+        <v>278</v>
+      </c>
+      <c r="ES1" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="EP1" s="11" t="s">
+      <c r="ET1" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="EQ1" s="13" t="s">
+      <c r="EU1" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="ER1" s="13" t="s">
+      <c r="EV1" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="ES1" s="13" t="s">
+      <c r="EW1" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="ET1" s="10" t="s">
+      <c r="EX1" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="EU1" s="10" t="s">
+      <c r="EY1" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="EV1" s="10" t="s">
+      <c r="EZ1" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="EW1" s="17" t="s">
+      <c r="FA1" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="EX1" s="10" t="s">
+      <c r="FB1" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="EY1" s="17" t="s">
+      <c r="FC1" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="EZ1" s="10" t="s">
+      <c r="FD1" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="FA1" s="10" t="s">
+      <c r="FE1" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="FB1" s="17" t="s">
+      <c r="FF1" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="FC1" s="13" t="s">
+      <c r="FG1" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="FD1" s="19" t="s">
+      <c r="FH1" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="FE1" s="20" t="s">
+      <c r="FI1" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="FF1" s="20" t="s">
+      <c r="FJ1" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="FG1" s="20" t="s">
+      <c r="FK1" s="20" t="s">
         <v>256</v>
       </c>
-      <c r="FH1" s="20" t="s">
+      <c r="FL1" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="FI1" s="20" t="s">
+      <c r="FM1" s="20" t="s">
         <v>260</v>
       </c>
-      <c r="FJ1" s="19" t="s">
+      <c r="FN1" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="FK1" s="20" t="s">
+      <c r="FO1" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="FL1" s="21" t="s">
+      <c r="FP1" s="21" t="s">
         <v>237</v>
       </c>
-      <c r="FM1" s="21" t="s">
+      <c r="FQ1" s="21" t="s">
         <v>238</v>
       </c>
-      <c r="FN1" s="21" t="s">
+      <c r="FR1" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="FO1" s="21" t="s">
+      <c r="FS1" s="21" t="s">
         <v>240</v>
       </c>
-      <c r="FP1" s="21" t="s">
+      <c r="FT1" s="21" t="s">
         <v>253</v>
       </c>
-      <c r="FQ1" s="22" t="s">
+      <c r="FU1" s="22" t="s">
         <v>241</v>
       </c>
-      <c r="FR1" s="22" t="s">
+      <c r="FV1" s="22" t="s">
         <v>242</v>
       </c>
-      <c r="FS1" s="22" t="s">
+      <c r="FW1" s="22" t="s">
         <v>243</v>
       </c>
-      <c r="FT1" s="22" t="s">
+      <c r="FX1" s="22" t="s">
         <v>244</v>
       </c>
-      <c r="FU1" s="22" t="s">
+      <c r="FY1" s="22" t="s">
         <v>254</v>
       </c>
-      <c r="FV1" s="21" t="s">
+      <c r="FZ1" s="21" t="s">
         <v>245</v>
       </c>
-      <c r="FW1" s="21" t="s">
+      <c r="GA1" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="FX1" s="21" t="s">
+      <c r="GB1" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="FY1" s="21" t="s">
+      <c r="GC1" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="FZ1" s="21" t="s">
+      <c r="GD1" s="21" t="s">
         <v>255</v>
       </c>
-      <c r="GA1" s="23" t="s">
+      <c r="GE1" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="GB1" s="23" t="s">
+      <c r="GF1" s="23" t="s">
         <v>172</v>
       </c>
-      <c r="GC1" s="23" t="s">
+      <c r="GG1" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="GD1" s="23" t="s">
+      <c r="GH1" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="GE1" s="24" t="s">
+      <c r="GI1" s="24" t="s">
         <v>175</v>
       </c>
-      <c r="GF1" s="23" t="s">
+      <c r="GJ1" s="23" t="s">
         <v>176</v>
       </c>
-      <c r="GG1" s="23" t="s">
+      <c r="GK1" s="23" t="s">
         <v>177</v>
       </c>
-      <c r="GH1" s="23" t="s">
+      <c r="GL1" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="GI1" s="23" t="s">
+      <c r="GM1" s="23" t="s">
         <v>179</v>
       </c>
-      <c r="GJ1" s="23" t="s">
+      <c r="GN1" s="23" t="s">
         <v>261</v>
       </c>
-      <c r="GK1" s="23" t="s">
+      <c r="GO1" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="GL1" s="23" t="s">
+      <c r="GP1" s="23" t="s">
         <v>180</v>
       </c>
-      <c r="GM1" s="23" t="s">
+      <c r="GQ1" s="23" t="s">
         <v>181</v>
       </c>
-      <c r="GN1" s="23" t="s">
+      <c r="GR1" s="23" t="s">
         <v>182</v>
       </c>
-      <c r="GO1" s="23" t="s">
+      <c r="GS1" s="23" t="s">
         <v>183</v>
       </c>
-      <c r="GP1" s="23" t="s">
+      <c r="GT1" s="23" t="s">
         <v>184</v>
       </c>
-      <c r="GQ1" s="23" t="s">
+      <c r="GU1" s="23" t="s">
         <v>185</v>
       </c>
-      <c r="GR1" s="24" t="s">
+      <c r="GV1" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="GS1" s="23" t="s">
+      <c r="GW1" s="23" t="s">
         <v>187</v>
       </c>
-      <c r="GT1" s="23" t="s">
+      <c r="GX1" s="23" t="s">
         <v>188</v>
       </c>
-      <c r="GU1" s="23" t="s">
+      <c r="GY1" s="23" t="s">
         <v>189</v>
       </c>
-      <c r="GV1" s="23" t="s">
+      <c r="GZ1" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="GW1" s="23" t="s">
+      <c r="HA1" s="23" t="s">
         <v>263</v>
       </c>
-      <c r="GX1" s="23" t="s">
+      <c r="HB1" s="23" t="s">
         <v>264</v>
       </c>
-      <c r="GY1" s="23" t="s">
+      <c r="HC1" s="23" t="s">
         <v>191</v>
       </c>
-      <c r="GZ1" s="23" t="s">
+      <c r="HD1" s="23" t="s">
         <v>192</v>
       </c>
-      <c r="HA1" s="23" t="s">
+      <c r="HE1" s="23" t="s">
         <v>193</v>
       </c>
-      <c r="HB1" s="23" t="s">
+      <c r="HF1" s="23" t="s">
         <v>194</v>
       </c>
-      <c r="HC1" s="23" t="s">
+      <c r="HG1" s="23" t="s">
         <v>195</v>
       </c>
-      <c r="HD1" s="23" t="s">
+      <c r="HH1" s="23" t="s">
         <v>196</v>
       </c>
-      <c r="HE1" s="24" t="s">
+      <c r="HI1" s="24" t="s">
         <v>197</v>
       </c>
-      <c r="HF1" s="23" t="s">
+      <c r="HJ1" s="23" t="s">
         <v>198</v>
       </c>
-      <c r="HG1" s="23" t="s">
+      <c r="HK1" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="HH1" s="23" t="s">
+      <c r="HL1" s="23" t="s">
         <v>200</v>
       </c>
-      <c r="HI1" s="23" t="s">
+      <c r="HM1" s="23" t="s">
         <v>201</v>
       </c>
-      <c r="HJ1" s="23" t="s">
+      <c r="HN1" s="23" t="s">
         <v>265</v>
       </c>
-      <c r="HK1" s="23" t="s">
+      <c r="HO1" s="23" t="s">
         <v>266</v>
       </c>
-      <c r="HL1" s="23" t="s">
+      <c r="HP1" s="23" t="s">
         <v>202</v>
       </c>
-      <c r="HM1" s="23" t="s">
+      <c r="HQ1" s="23" t="s">
         <v>203</v>
       </c>
-      <c r="HN1" s="23" t="s">
+      <c r="HR1" s="23" t="s">
         <v>204</v>
       </c>
-      <c r="HO1" s="23" t="s">
+      <c r="HS1" s="23" t="s">
         <v>205</v>
       </c>
-      <c r="HP1" s="23" t="s">
+      <c r="HT1" s="23" t="s">
         <v>206</v>
       </c>
-      <c r="HQ1" s="23" t="s">
+      <c r="HU1" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="HR1" s="24" t="s">
+      <c r="HV1" s="24" t="s">
         <v>208</v>
       </c>
-      <c r="HS1" s="23" t="s">
+      <c r="HW1" s="23" t="s">
         <v>209</v>
       </c>
-      <c r="HT1" s="23" t="s">
+      <c r="HX1" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="HU1" s="23" t="s">
+      <c r="HY1" s="23" t="s">
         <v>211</v>
       </c>
-      <c r="HV1" s="23" t="s">
+      <c r="HZ1" s="23" t="s">
         <v>212</v>
       </c>
-      <c r="HW1" s="23" t="s">
+      <c r="IA1" s="23" t="s">
         <v>267</v>
       </c>
-      <c r="HX1" s="23" t="s">
+      <c r="IB1" s="23" t="s">
         <v>268</v>
       </c>
-      <c r="HY1" s="23" t="s">
+      <c r="IC1" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="HZ1" s="23" t="s">
+      <c r="ID1" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="IA1" s="23" t="s">
+      <c r="IE1" s="23" t="s">
         <v>215</v>
       </c>
-      <c r="IB1" s="23" t="s">
+      <c r="IF1" s="23" t="s">
         <v>216</v>
       </c>
-      <c r="IC1" s="23" t="s">
+      <c r="IG1" s="23" t="s">
         <v>217</v>
       </c>
-      <c r="ID1" s="23" t="s">
+      <c r="IH1" s="23" t="s">
         <v>218</v>
       </c>
-      <c r="IE1" s="24" t="s">
+      <c r="II1" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="IF1" s="23" t="s">
+      <c r="IJ1" s="23" t="s">
         <v>220</v>
       </c>
-      <c r="IG1" s="23" t="s">
+      <c r="IK1" s="23" t="s">
         <v>221</v>
       </c>
-      <c r="IH1" s="23" t="s">
+      <c r="IL1" s="23" t="s">
         <v>222</v>
       </c>
-      <c r="II1" s="23" t="s">
+      <c r="IM1" s="23" t="s">
         <v>223</v>
       </c>
-      <c r="IJ1" s="23" t="s">
+      <c r="IN1" s="23" t="s">
         <v>269</v>
       </c>
-      <c r="IK1" s="23" t="s">
+      <c r="IO1" s="23" t="s">
         <v>270</v>
       </c>
-      <c r="IL1" s="23" t="s">
+      <c r="IP1" s="23" t="s">
         <v>224</v>
       </c>
-      <c r="IM1" s="23" t="s">
+      <c r="IQ1" s="23" t="s">
         <v>225</v>
       </c>
-      <c r="IN1" s="23" t="s">
+      <c r="IR1" s="23" t="s">
         <v>226</v>
       </c>
-      <c r="IO1" s="23" t="s">
+      <c r="IS1" s="23" t="s">
         <v>227</v>
       </c>
-      <c r="IP1" s="23" t="s">
+      <c r="IT1" s="23" t="s">
         <v>228</v>
       </c>
-      <c r="IQ1" s="23" t="s">
+      <c r="IU1" s="23" t="s">
         <v>229</v>
       </c>
-      <c r="IR1" s="24" t="s">
+      <c r="IV1" s="24" t="s">
         <v>230</v>
       </c>
-      <c r="IS1" s="23" t="s">
+      <c r="IW1" s="23" t="s">
         <v>231</v>
       </c>
-      <c r="IT1" s="23" t="s">
+      <c r="IX1" s="23" t="s">
         <v>232</v>
       </c>
-      <c r="IU1" s="23" t="s">
+      <c r="IY1" s="23" t="s">
         <v>233</v>
       </c>
-      <c r="IV1" s="23" t="s">
+      <c r="IZ1" s="23" t="s">
         <v>234</v>
       </c>
-      <c r="IW1" s="23" t="s">
+      <c r="JA1" s="23" t="s">
         <v>271</v>
       </c>
-      <c r="IX1" s="23" t="s">
+      <c r="JB1" s="23" t="s">
         <v>272</v>
       </c>
-      <c r="IY1" s="23" t="s">
+      <c r="JC1" s="23" t="s">
         <v>235</v>
       </c>
-      <c r="IZ1" s="23" t="s">
+      <c r="JD1" s="23" t="s">
         <v>236</v>
       </c>
-      <c r="JA1" s="25" t="s">
+      <c r="JE1" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="JB1" s="25" t="s">
+      <c r="JF1" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="JC1" s="25" t="s">
+      <c r="JG1" s="25" t="s">
         <v>133</v>
       </c>
-      <c r="JD1" s="25" t="s">
+      <c r="JH1" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="JE1" s="25" t="s">
+      <c r="JI1" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="JF1" s="25" t="s">
+      <c r="JJ1" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="JG1" s="25" t="s">
+      <c r="JK1" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="JH1" s="25" t="s">
+      <c r="JL1" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="JI1" s="25" t="s">
+      <c r="JM1" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="JJ1" s="25" t="s">
+      <c r="JN1" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="JK1" s="25" t="s">
+      <c r="JO1" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="JL1" s="25" t="s">
+      <c r="JP1" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="JM1" s="25" t="s">
+      <c r="JQ1" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="JN1" s="10" t="s">
+      <c r="JR1" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="JO1" s="10" t="s">
+      <c r="JS1" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="JP1" s="10" t="s">
+      <c r="JT1" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="JQ1" s="10" t="s">
+      <c r="JU1" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="JR1" s="10" t="s">
+      <c r="JV1" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="JS1" s="10" t="s">
+      <c r="JW1" s="10" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="3" spans="1:279" x14ac:dyDescent="0.25">
-      <c r="FS3" s="2"/>
-      <c r="FT3" s="2"/>
-      <c r="FU3" s="2"/>
+    <row r="3" spans="1:283" x14ac:dyDescent="0.25">
+      <c r="FW3" s="2"/>
+      <c r="FX3" s="2"/>
+      <c r="FY3" s="2"/>
     </row>
-    <row r="5" spans="1:279" x14ac:dyDescent="0.25">
-      <c r="GE5" s="9"/>
-      <c r="GF5" s="7"/>
+    <row r="5" spans="1:283" x14ac:dyDescent="0.25">
+      <c r="GI5" s="9"/>
+      <c r="GJ5" s="7"/>
     </row>
-    <row r="6" spans="1:279" x14ac:dyDescent="0.25">
-      <c r="GE6" s="9"/>
-      <c r="GF6" s="7"/>
+    <row r="6" spans="1:283" x14ac:dyDescent="0.25">
+      <c r="GI6" s="9"/>
+      <c r="GJ6" s="7"/>
     </row>
-    <row r="7" spans="1:279" x14ac:dyDescent="0.25">
-      <c r="GE7" s="9"/>
-      <c r="GF7" s="7"/>
+    <row r="7" spans="1:283" x14ac:dyDescent="0.25">
+      <c r="GI7" s="9"/>
+      <c r="GJ7" s="7"/>
     </row>
-    <row r="8" spans="1:279" x14ac:dyDescent="0.25">
-      <c r="GE8" s="9"/>
-      <c r="GF8" s="7"/>
-      <c r="GR8" s="7"/>
-      <c r="GS8" s="7"/>
-      <c r="HE8" s="7"/>
-      <c r="HF8" s="7"/>
-      <c r="HR8" s="7"/>
-      <c r="HS8" s="7"/>
-      <c r="IE8" s="7"/>
-      <c r="IF8" s="7"/>
-      <c r="IR8" s="7"/>
-      <c r="IS8" s="7"/>
+    <row r="8" spans="1:283" x14ac:dyDescent="0.25">
+      <c r="GI8" s="9"/>
+      <c r="GJ8" s="7"/>
+      <c r="GV8" s="7"/>
+      <c r="GW8" s="7"/>
+      <c r="HI8" s="7"/>
+      <c r="HJ8" s="7"/>
+      <c r="HV8" s="7"/>
+      <c r="HW8" s="7"/>
+      <c r="II8" s="7"/>
+      <c r="IJ8" s="7"/>
+      <c r="IV8" s="7"/>
+      <c r="IW8" s="7"/>
     </row>
-    <row r="9" spans="1:279" x14ac:dyDescent="0.25">
-      <c r="GE9" s="9"/>
-      <c r="GF9" s="7"/>
+    <row r="9" spans="1:283" x14ac:dyDescent="0.25">
+      <c r="GI9" s="9"/>
+      <c r="GJ9" s="7"/>
     </row>
-    <row r="10" spans="1:279" x14ac:dyDescent="0.25">
-      <c r="GE10" s="9"/>
-      <c r="GF10" s="7"/>
+    <row r="10" spans="1:283" x14ac:dyDescent="0.25">
+      <c r="GI10" s="9"/>
+      <c r="GJ10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>